<commit_message>
removed 1386 mesh_topology from CR ; removed 442/410/409 from pub_index ; added 442/410/409 LF SCHEMAS's WG Numbers
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_Geometry/Bugzilla_list.xlsx
+++ b/publication/part1000/CR_Geometry/Bugzilla_list.xlsx
@@ -9,18 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="1200" yWindow="-18460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CR_geometry Bugs and Parts list" sheetId="1" r:id="rId1"/>
-    <sheet name="Bugs vs Parts Summary" sheetId="4" r:id="rId2"/>
-    <sheet name="Legend" sheetId="3" r:id="rId3"/>
-    <sheet name="Innitial collector bugs back up" sheetId="2" r:id="rId4"/>
+    <sheet name="Bugs vs Parts Summary" sheetId="6" r:id="rId2"/>
+    <sheet name="Moved out from initial list" sheetId="2" r:id="rId3"/>
+    <sheet name="Legend" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
-  <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="100">
   <si>
     <t>Bug Description</t>
   </si>
@@ -324,18 +321,6 @@
   </si>
   <si>
     <t>Bugs</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Count of Parts</t>
-  </si>
-  <si>
-    <t>Number Of  Parts in CR_Geometry</t>
   </si>
   <si>
     <t xml:space="preserve">description file for scan_data_3d_shape_model_schema is corrupt and prevent build </t>
@@ -351,7 +336,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -390,25 +375,13 @@
       <color theme="5" tint="-0.499984740745262"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -425,7 +398,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -434,23 +407,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -458,52 +414,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <strike val="0"/>
@@ -702,6 +613,45 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
   </dxfs>
@@ -714,804 +664,29 @@
 </styleSheet>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Kevin Le Tutour" refreshedDate="42472.822082638886" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="66">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="C1:D69" sheet="CR_geometry Bugs and Parts list"/>
-  </cacheSource>
-  <cacheFields count="2">
-    <cacheField name="Parts" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="42" maxValue="1831" count="33">
-        <n v="42"/>
-        <n v="43"/>
-        <n v="409"/>
-        <n v="410"/>
-        <n v="442"/>
-        <n v="1004"/>
-        <n v="1005"/>
-        <n v="1110"/>
-        <n v="1131"/>
-        <n v="1318"/>
-        <n v="1319"/>
-        <n v="1386"/>
-        <n v="1507"/>
-        <n v="1509"/>
-        <n v="1514"/>
-        <n v="1520"/>
-        <n v="1521"/>
-        <n v="1522"/>
-        <n v="1523"/>
-        <n v="1525"/>
-        <n v="1652"/>
-        <n v="1702"/>
-        <n v="1731"/>
-        <n v="1767"/>
-        <n v="1789"/>
-        <n v="1790"/>
-        <n v="1791"/>
-        <n v="1792"/>
-        <n v="1813"/>
-        <n v="1819"/>
-        <n v="1820"/>
-        <n v="1830"/>
-        <n v="1831"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Bugs" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4853" maxValue="5900" count="38">
-        <n v="5409"/>
-        <n v="5448"/>
-        <n v="5452"/>
-        <n v="5527"/>
-        <n v="5566"/>
-        <n v="4861"/>
-        <n v="5703"/>
-        <n v="5650"/>
-        <n v="5805"/>
-        <n v="5454"/>
-        <n v="5898"/>
-        <n v="5897"/>
-        <n v="5896"/>
-        <n v="5605"/>
-        <n v="5151"/>
-        <n v="5662"/>
-        <n v="5465"/>
-        <n v="5217"/>
-        <n v="5554"/>
-        <n v="5030"/>
-        <n v="5509"/>
-        <n v="4987"/>
-        <n v="5673"/>
-        <n v="5630"/>
-        <n v="4853"/>
-        <n v="5653"/>
-        <n v="4914"/>
-        <n v="5458"/>
-        <n v="5526"/>
-        <n v="5550"/>
-        <n v="5677"/>
-        <n v="5623"/>
-        <n v="5900"/>
-        <n v="5434"/>
-        <n v="5595"/>
-        <n v="5596"/>
-        <n v="5891"/>
-        <n v="5528"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="66">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="17"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <x v="20"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <x v="21"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="12"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="23"/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="16"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="17"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="20"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="22"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="23"/>
-    <x v="24"/>
-  </r>
-  <r>
-    <x v="23"/>
-    <x v="25"/>
-  </r>
-  <r>
-    <x v="23"/>
-    <x v="26"/>
-  </r>
-  <r>
-    <x v="24"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="24"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="25"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="25"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="26"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="27"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="28"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <x v="27"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <x v="28"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <x v="29"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <x v="30"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <x v="31"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <x v="32"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="30"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="31"/>
-    <x v="33"/>
-  </r>
-  <r>
-    <x v="31"/>
-    <x v="34"/>
-  </r>
-  <r>
-    <x v="31"/>
-    <x v="35"/>
-  </r>
-  <r>
-    <x v="31"/>
-    <x v="36"/>
-  </r>
-  <r>
-    <x v="31"/>
-    <x v="32"/>
-  </r>
-  <r>
-    <x v="32"/>
-    <x v="37"/>
-  </r>
-  <r>
-    <x v="32"/>
-    <x v="32"/>
-  </r>
-  <r>
-    <x v="32"/>
-    <x v="15"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B103" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="34">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="39">
-        <item x="24"/>
-        <item x="5"/>
-        <item x="26"/>
-        <item x="21"/>
-        <item x="19"/>
-        <item x="14"/>
-        <item x="17"/>
-        <item x="0"/>
-        <item x="33"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="9"/>
-        <item x="27"/>
-        <item x="16"/>
-        <item x="20"/>
-        <item x="28"/>
-        <item x="3"/>
-        <item x="37"/>
-        <item x="29"/>
-        <item x="18"/>
-        <item x="4"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="13"/>
-        <item x="31"/>
-        <item x="23"/>
-        <item x="7"/>
-        <item x="25"/>
-        <item x="15"/>
-        <item x="22"/>
-        <item x="30"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="36"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="10"/>
-        <item x="32"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="100">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="26"/>
-    </i>
-    <i r="1">
-      <x v="31"/>
-    </i>
-    <i r="1">
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="23"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="24"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
-    </i>
-    <i r="1">
-      <x v="30"/>
-    </i>
-    <i r="1">
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
-    </i>
-    <i r="1">
-      <x v="33"/>
-    </i>
-    <i r="1">
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
-    </i>
-    <i r="1">
-      <x v="37"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Parts" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="3">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P72" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:P72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P67" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:P67"/>
   <sortState ref="A2:P67">
     <sortCondition ref="C1:C67"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="Status key" dataDxfId="16"/>
-    <tableColumn id="2" name="Status" dataDxfId="15"/>
-    <tableColumn id="3" name="Parts" dataDxfId="14"/>
-    <tableColumn id="4" name="Bugs" dataDxfId="13"/>
-    <tableColumn id="5" name="Bug Description" dataDxfId="12"/>
-    <tableColumn id="6" name="checked if last BZ comments consistent" dataDxfId="11"/>
-    <tableColumn id="7" name="moved to CR_Geometry milestone" dataDxfId="10"/>
-    <tableColumn id="8" name="in publication index" dataDxfId="9"/>
-    <tableColumn id="9" name="bugs in the publication index" dataDxfId="8"/>
-    <tableColumn id="10" name="stepmod changes done locally" dataDxfId="7"/>
-    <tableColumn id="11" name="checked if other bugs against this module from CR11" dataDxfId="2"/>
-    <tableColumn id="12" name="checked date format " dataDxfId="0"/>
-    <tableColumn id="13" name="check change history" dataDxfId="1"/>
-    <tableColumn id="14" name="changes committed and tagged" dataDxfId="6"/>
-    <tableColumn id="16" name="WG NB updated" dataDxfId="5"/>
-    <tableColumn id="15" name="publication date updated and " dataDxfId="4"/>
+    <tableColumn id="1" name="Status key" dataDxfId="15"/>
+    <tableColumn id="2" name="Status" dataDxfId="14"/>
+    <tableColumn id="3" name="Parts" dataDxfId="13"/>
+    <tableColumn id="4" name="Bugs" dataDxfId="12"/>
+    <tableColumn id="5" name="Bug Description" dataDxfId="11"/>
+    <tableColumn id="6" name="checked if last BZ comments consistent" dataDxfId="10"/>
+    <tableColumn id="7" name="moved to CR_Geometry milestone" dataDxfId="9"/>
+    <tableColumn id="8" name="in publication index" dataDxfId="8"/>
+    <tableColumn id="9" name="bugs in the publication index" dataDxfId="7"/>
+    <tableColumn id="10" name="stepmod changes done locally" dataDxfId="6"/>
+    <tableColumn id="11" name="checked if other bugs against this module from CR11" dataDxfId="5"/>
+    <tableColumn id="12" name="checked date format " dataDxfId="4"/>
+    <tableColumn id="13" name="check change history" dataDxfId="3"/>
+    <tableColumn id="14" name="changes committed and tagged" dataDxfId="2"/>
+    <tableColumn id="16" name="WG NB updated" dataDxfId="1"/>
+    <tableColumn id="15" name="publication date updated and " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1780,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1791,7 +966,7 @@
     <col min="1" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="59.83203125" customWidth="1"/>
     <col min="6" max="11" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="6" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" customWidth="1"/>
     <col min="14" max="14" width="11.6640625" customWidth="1"/>
     <col min="15" max="16" width="10.6640625" customWidth="1"/>
@@ -2045,7 +1220,7 @@
         <v>5566</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>19</v>
@@ -2275,7 +1450,7 @@
         <v>5650</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>12</v>
@@ -2979,7 +2154,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -3022,37 +2197,39 @@
       <c r="P28" s="1"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>0</v>
+      <c r="A29" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1386</v>
-      </c>
-      <c r="D29" s="2">
-        <v>4987</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>52</v>
+        <v>28</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1507</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5554</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K29" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="L29" s="1" t="s">
         <v>12</v>
       </c>
@@ -3062,20 +2239,20 @@
       <c r="P29" s="1"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>3</v>
+      <c r="A30" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1386</v>
-      </c>
-      <c r="D30" s="2">
-        <v>5673</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1509</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5554</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>12</v>
@@ -3087,7 +2264,7 @@
         <v>12</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>12</v>
@@ -3111,7 +2288,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="1">
-        <v>1507</v>
+        <v>1514</v>
       </c>
       <c r="D31" s="1">
         <v>5554</v>
@@ -3146,20 +2323,20 @@
       <c r="P31" s="1"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>16</v>
+      <c r="A32" s="1">
+        <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1">
-        <v>1509</v>
+        <v>1520</v>
       </c>
       <c r="D32" s="1">
-        <v>5554</v>
+        <v>5630</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>12</v>
@@ -3171,7 +2348,7 @@
         <v>12</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>12</v>
@@ -3182,10 +2359,14 @@
       <c r="L32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="1"/>
+      <c r="M32" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
+      <c r="P32" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
@@ -3195,7 +2376,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="1">
-        <v>1514</v>
+        <v>1520</v>
       </c>
       <c r="D33" s="1">
         <v>5554</v>
@@ -3213,7 +2394,7 @@
         <v>12</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>12</v>
@@ -3224,26 +2405,30 @@
       <c r="L33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M33" s="1"/>
+      <c r="M33" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
+      <c r="P33" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>3</v>
+      <c r="A34" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D34" s="1">
-        <v>5630</v>
+        <v>5554</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>12</v>
@@ -3255,7 +2440,7 @@
         <v>12</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>12</v>
@@ -3266,14 +2451,10 @@
       <c r="L34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M34" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="P34" s="1"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -3283,7 +2464,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="1">
-        <v>1520</v>
+        <v>1522</v>
       </c>
       <c r="D35" s="1">
         <v>5554</v>
@@ -3301,25 +2482,21 @@
         <v>12</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M35" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="P35" s="1"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
@@ -3329,7 +2506,7 @@
         <v>28</v>
       </c>
       <c r="C36" s="1">
-        <v>1521</v>
+        <v>1523</v>
       </c>
       <c r="D36" s="1">
         <v>5554</v>
@@ -3371,7 +2548,7 @@
         <v>28</v>
       </c>
       <c r="C37" s="1">
-        <v>1522</v>
+        <v>1525</v>
       </c>
       <c r="D37" s="1">
         <v>5554</v>
@@ -3395,7 +2572,7 @@
         <v>12</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>12</v>
@@ -3413,7 +2590,7 @@
         <v>28</v>
       </c>
       <c r="C38" s="1">
-        <v>1523</v>
+        <v>1652</v>
       </c>
       <c r="D38" s="1">
         <v>5554</v>
@@ -3455,7 +2632,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="1">
-        <v>1525</v>
+        <v>1702</v>
       </c>
       <c r="D39" s="1">
         <v>5554</v>
@@ -3497,7 +2674,7 @@
         <v>28</v>
       </c>
       <c r="C40" s="1">
-        <v>1652</v>
+        <v>1731</v>
       </c>
       <c r="D40" s="1">
         <v>5554</v>
@@ -3533,19 +2710,19 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C41" s="1">
-        <v>1702</v>
+        <v>1767</v>
       </c>
       <c r="D41" s="1">
-        <v>5554</v>
+        <v>4853</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>12</v>
@@ -3557,7 +2734,7 @@
         <v>12</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>12</v>
@@ -3578,16 +2755,16 @@
         <v>16</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C42" s="1">
-        <v>1731</v>
+        <v>1767</v>
       </c>
       <c r="D42" s="1">
-        <v>5554</v>
+        <v>5653</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>12</v>
@@ -3599,7 +2776,7 @@
         <v>12</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>12</v>
@@ -3617,19 +2794,19 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C43" s="1">
         <v>1767</v>
       </c>
       <c r="D43" s="1">
-        <v>4853</v>
+        <v>4914</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>12</v>
@@ -3662,16 +2839,16 @@
         <v>16</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C44" s="1">
-        <v>1767</v>
+        <v>1789</v>
       </c>
       <c r="D44" s="1">
-        <v>5653</v>
+        <v>5554</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>12</v>
@@ -3683,7 +2860,7 @@
         <v>12</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>12</v>
@@ -3704,16 +2881,16 @@
         <v>16</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C45" s="1">
-        <v>1767</v>
+        <v>1789</v>
       </c>
       <c r="D45" s="1">
-        <v>4914</v>
+        <v>5662</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>12</v>
@@ -3725,7 +2902,7 @@
         <v>12</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>12</v>
@@ -3749,7 +2926,7 @@
         <v>28</v>
       </c>
       <c r="C46" s="1">
-        <v>1789</v>
+        <v>1790</v>
       </c>
       <c r="D46" s="1">
         <v>5554</v>
@@ -3791,7 +2968,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="1">
-        <v>1789</v>
+        <v>1790</v>
       </c>
       <c r="D47" s="1">
         <v>5662</v>
@@ -3833,7 +3010,7 @@
         <v>28</v>
       </c>
       <c r="C48" s="1">
-        <v>1790</v>
+        <v>1791</v>
       </c>
       <c r="D48" s="1">
         <v>5554</v>
@@ -3851,7 +3028,7 @@
         <v>12</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>12</v>
@@ -3875,13 +3052,13 @@
         <v>28</v>
       </c>
       <c r="C49" s="1">
-        <v>1790</v>
+        <v>1792</v>
       </c>
       <c r="D49" s="1">
-        <v>5662</v>
+        <v>5554</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>12</v>
@@ -3893,7 +3070,7 @@
         <v>12</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>12</v>
@@ -3917,7 +3094,7 @@
         <v>28</v>
       </c>
       <c r="C50" s="1">
-        <v>1791</v>
+        <v>1813</v>
       </c>
       <c r="D50" s="1">
         <v>5554</v>
@@ -3953,19 +3130,19 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C51" s="1">
-        <v>1792</v>
+        <v>1819</v>
       </c>
       <c r="D51" s="1">
-        <v>5554</v>
+        <v>5458</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>12</v>
@@ -3977,7 +3154,7 @@
         <v>12</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>12</v>
@@ -3991,23 +3168,25 @@
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
+      <c r="P51" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C52" s="1">
-        <v>1813</v>
+        <v>1819</v>
       </c>
       <c r="D52" s="1">
-        <v>5554</v>
+        <v>5526</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>12</v>
@@ -4019,7 +3198,7 @@
         <v>12</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>12</v>
@@ -4033,23 +3212,25 @@
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
+      <c r="P52" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>36</v>
+      <c r="A53" s="1">
+        <v>3</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="C53" s="1">
         <v>1819</v>
       </c>
       <c r="D53" s="1">
-        <v>5458</v>
+        <v>5550</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>12</v>
@@ -4080,20 +3261,20 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>39</v>
+      <c r="A54" s="1">
+        <v>3</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C54" s="1">
         <v>1819</v>
       </c>
       <c r="D54" s="1">
-        <v>5526</v>
+        <v>5677</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>12</v>
@@ -4124,20 +3305,20 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>3</v>
+      <c r="A55" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C55" s="1">
         <v>1819</v>
       </c>
       <c r="D55" s="1">
-        <v>5550</v>
+        <v>5623</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>12</v>
@@ -4168,20 +3349,20 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>3</v>
+      <c r="A56" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C56" s="1">
         <v>1819</v>
       </c>
       <c r="D56" s="1">
-        <v>5677</v>
+        <v>5554</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>12</v>
@@ -4216,16 +3397,16 @@
         <v>16</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C57" s="1">
         <v>1819</v>
       </c>
       <c r="D57" s="1">
-        <v>5623</v>
+        <v>5900</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>12</v>
@@ -4266,10 +3447,10 @@
         <v>1819</v>
       </c>
       <c r="D58" s="1">
-        <v>5554</v>
+        <v>5662</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>12</v>
@@ -4304,16 +3485,16 @@
         <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C59" s="1">
-        <v>1819</v>
+        <v>1820</v>
       </c>
       <c r="D59" s="1">
-        <v>5900</v>
+        <v>5554</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>12</v>
@@ -4339,28 +3520,26 @@
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
-      <c r="P59" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="P59" s="1"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>16</v>
+      <c r="A60" s="1">
+        <v>3</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C60" s="1">
-        <v>1819</v>
+        <v>1830</v>
       </c>
       <c r="D60" s="1">
-        <v>5662</v>
+        <v>5434</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>12</v>
@@ -4374,9 +3553,7 @@
       <c r="J60" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K60" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="K60" s="1"/>
       <c r="L60" s="1" t="s">
         <v>12</v>
       </c>
@@ -4388,20 +3565,20 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>16</v>
+      <c r="A61" s="1">
+        <v>3</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C61" s="1">
-        <v>1820</v>
+        <v>1830</v>
       </c>
       <c r="D61" s="1">
-        <v>5554</v>
+        <v>5595</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>12</v>
@@ -4427,7 +3604,9 @@
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
+      <c r="P61" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
@@ -4440,13 +3619,13 @@
         <v>1830</v>
       </c>
       <c r="D62" s="1">
-        <v>5434</v>
+        <v>5596</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>12</v>
@@ -4472,20 +3651,20 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
-        <v>3</v>
+      <c r="A63" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C63" s="1">
         <v>1830</v>
       </c>
       <c r="D63" s="1">
-        <v>5595</v>
+        <v>5891</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>12</v>
@@ -4516,20 +3695,20 @@
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
-        <v>3</v>
+      <c r="A64" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C64" s="1">
         <v>1830</v>
       </c>
       <c r="D64" s="1">
-        <v>5596</v>
+        <v>5900</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>12</v>
@@ -4546,7 +3725,9 @@
       <c r="J64" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K64" s="1"/>
+      <c r="K64" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="L64" s="1" t="s">
         <v>12</v>
       </c>
@@ -4558,23 +3739,23 @@
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>16</v>
+      <c r="A65" s="1">
+        <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C65" s="1">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="D65" s="1">
-        <v>5891</v>
+        <v>5528</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>12</v>
@@ -4583,7 +3764,7 @@
         <v>12</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>12</v>
@@ -4609,7 +3790,7 @@
         <v>21</v>
       </c>
       <c r="C66" s="1">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="D66" s="1">
         <v>5900</v>
@@ -4627,7 +3808,7 @@
         <v>12</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>12</v>
@@ -4646,23 +3827,23 @@
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
-        <v>0</v>
+      <c r="A67" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C67" s="1">
         <v>1831</v>
       </c>
       <c r="D67" s="1">
-        <v>5528</v>
+        <v>5662</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>12</v>
@@ -4688,148 +3869,6 @@
       <c r="P67" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C68" s="1">
-        <v>1831</v>
-      </c>
-      <c r="D68" s="1">
-        <v>5900</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C69" s="1">
-        <v>1831</v>
-      </c>
-      <c r="D69" s="1">
-        <v>5662</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4842,844 +3881,181 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B104"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
-    <col min="3" max="38" width="15.5" style="1" customWidth="1"/>
-    <col min="39" max="40" width="10.6640625" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="43.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="99.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>97</v>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1">
+        <v>5554</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5644</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>42</v>
-      </c>
-      <c r="B4" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
-        <v>4861</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
-        <v>5409</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
-        <v>5448</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
-        <v>5452</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
-        <v>5527</v>
-      </c>
-      <c r="B9" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>5566</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>5650</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>5703</v>
-      </c>
-      <c r="B12" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5805</v>
-      </c>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
-        <v>43</v>
-      </c>
-      <c r="B14" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>5454</v>
-      </c>
-      <c r="B15" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
-        <v>409</v>
-      </c>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>5898</v>
-      </c>
-      <c r="B17" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
-        <v>410</v>
-      </c>
-      <c r="B18" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
-        <v>5897</v>
-      </c>
-      <c r="B19" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>442</v>
-      </c>
-      <c r="B20" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
-        <v>5896</v>
-      </c>
-      <c r="B21" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
-        <v>1004</v>
-      </c>
-      <c r="B22" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="9">
-        <v>5151</v>
-      </c>
-      <c r="B23" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="9">
-        <v>5217</v>
-      </c>
-      <c r="B24" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="9">
-        <v>5465</v>
-      </c>
-      <c r="B25" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
-        <v>5605</v>
-      </c>
-      <c r="B26" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="9">
+        <v>73</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="1">
         <v>5662</v>
       </c>
-      <c r="B27" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
-        <v>1005</v>
-      </c>
-      <c r="B28" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B29" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="9">
-        <v>5662</v>
-      </c>
-      <c r="B30" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
-        <v>1110</v>
-      </c>
-      <c r="B31" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B32" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
-        <v>1131</v>
-      </c>
-      <c r="B33" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="9">
-        <v>5030</v>
-      </c>
-      <c r="B34" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B35" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
-        <v>1318</v>
-      </c>
-      <c r="B36" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="9">
-        <v>5509</v>
-      </c>
-      <c r="B37" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
-        <v>1319</v>
-      </c>
-      <c r="B38" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="9">
-        <v>5662</v>
-      </c>
-      <c r="B39" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2">
         <v>1386</v>
       </c>
-      <c r="B40" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="9">
+      <c r="D4" s="2">
         <v>4987</v>
       </c>
-      <c r="B41" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="9">
+      <c r="E4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1386</v>
+      </c>
+      <c r="D5" s="2">
         <v>5673</v>
       </c>
-      <c r="B42" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
-        <v>1507</v>
-      </c>
-      <c r="B43" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B44" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="7">
-        <v>1509</v>
-      </c>
-      <c r="B45" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B46" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
-        <v>1514</v>
-      </c>
-      <c r="B47" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B48" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7">
-        <v>1520</v>
-      </c>
-      <c r="B49" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B50" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="9">
-        <v>5630</v>
-      </c>
-      <c r="B51" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7">
-        <v>1521</v>
-      </c>
-      <c r="B52" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B53" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="7">
-        <v>1522</v>
-      </c>
-      <c r="B54" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B55" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="7">
-        <v>1523</v>
-      </c>
-      <c r="B56" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B57" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="7">
-        <v>1525</v>
-      </c>
-      <c r="B58" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B59" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="7">
-        <v>1652</v>
-      </c>
-      <c r="B60" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B61" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="7">
-        <v>1702</v>
-      </c>
-      <c r="B62" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B63" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="7">
-        <v>1731</v>
-      </c>
-      <c r="B64" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B65" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="7">
-        <v>1767</v>
-      </c>
-      <c r="B66" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="9">
-        <v>4853</v>
-      </c>
-      <c r="B67" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="9">
-        <v>4914</v>
-      </c>
-      <c r="B68" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="9">
-        <v>5653</v>
-      </c>
-      <c r="B69" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="7">
-        <v>1789</v>
-      </c>
-      <c r="B70" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B71" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="9">
-        <v>5662</v>
-      </c>
-      <c r="B72" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="7">
-        <v>1790</v>
-      </c>
-      <c r="B73" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B74" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="9">
-        <v>5662</v>
-      </c>
-      <c r="B75" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="7">
-        <v>1791</v>
-      </c>
-      <c r="B76" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B77" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="7">
-        <v>1792</v>
-      </c>
-      <c r="B78" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B79" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="7">
-        <v>1813</v>
-      </c>
-      <c r="B80" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B81" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="7">
-        <v>1819</v>
-      </c>
-      <c r="B82" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="9">
-        <v>5458</v>
-      </c>
-      <c r="B83" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="9">
-        <v>5526</v>
-      </c>
-      <c r="B84" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="9">
-        <v>5550</v>
-      </c>
-      <c r="B85" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B86" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="9">
-        <v>5623</v>
-      </c>
-      <c r="B87" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="9">
-        <v>5662</v>
-      </c>
-      <c r="B88" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="9">
-        <v>5677</v>
-      </c>
-      <c r="B89" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="9">
-        <v>5900</v>
-      </c>
-      <c r="B90" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="7">
-        <v>1820</v>
-      </c>
-      <c r="B91" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="9">
-        <v>5554</v>
-      </c>
-      <c r="B92" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="7">
-        <v>1830</v>
-      </c>
-      <c r="B93" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="9">
-        <v>5434</v>
-      </c>
-      <c r="B94" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="9">
-        <v>5595</v>
-      </c>
-      <c r="B95" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="9">
-        <v>5596</v>
-      </c>
-      <c r="B96" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="9">
-        <v>5891</v>
-      </c>
-      <c r="B97" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="9">
-        <v>5900</v>
-      </c>
-      <c r="B98" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="7">
-        <v>1831</v>
-      </c>
-      <c r="B99" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="9">
-        <v>5528</v>
-      </c>
-      <c r="B100" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="9">
-        <v>5662</v>
-      </c>
-      <c r="B101" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="9">
-        <v>5900</v>
-      </c>
-      <c r="B102" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B103" s="8">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" s="12" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B104" s="11">
-        <f>GETPIVOTDATA("Parts",$A$3)/2</f>
-        <v>33</v>
-      </c>
+      <c r="E5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -5787,86 +4163,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="43.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="34.83203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="1">
-        <v>5554</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5644</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5662</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
final version of publication index
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_Geometry/Bugzilla_list.xlsx
+++ b/publication/part1000/CR_Geometry/Bugzilla_list.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="100">
   <si>
     <t>Bug Description</t>
   </si>
@@ -665,8 +665,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P67" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:P67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P68" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:P68"/>
   <sortState ref="A2:P67">
     <sortCondition ref="C1:C67"/>
   </sortState>
@@ -955,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2222,7 +2222,7 @@
         <v>12</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>12</v>
@@ -2243,16 +2243,16 @@
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C30" s="1">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="D30" s="1">
-        <v>5554</v>
+        <v>5662</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>12</v>
@@ -2264,7 +2264,7 @@
         <v>12</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>12</v>
@@ -2288,7 +2288,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="1">
-        <v>1514</v>
+        <v>1509</v>
       </c>
       <c r="D31" s="1">
         <v>5554</v>
@@ -2323,20 +2323,20 @@
       <c r="P31" s="1"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>3</v>
+      <c r="A32" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C32" s="1">
-        <v>1520</v>
+        <v>1514</v>
       </c>
       <c r="D32" s="1">
-        <v>5630</v>
+        <v>5554</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>12</v>
@@ -2348,7 +2348,7 @@
         <v>12</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>12</v>
@@ -2359,30 +2359,26 @@
       <c r="L32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="P32" s="1"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>16</v>
+      <c r="A33" s="1">
+        <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1">
         <v>1520</v>
       </c>
       <c r="D33" s="1">
-        <v>5554</v>
+        <v>5630</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>12</v>
@@ -2422,7 +2418,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="1">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="D34" s="1">
         <v>5554</v>
@@ -2440,7 +2436,7 @@
         <v>12</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>12</v>
@@ -2451,10 +2447,14 @@
       <c r="L34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M34" s="1"/>
+      <c r="M34" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
+      <c r="P34" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -2464,7 +2464,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="1">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="D35" s="1">
         <v>5554</v>
@@ -2488,7 +2488,7 @@
         <v>12</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>12</v>
@@ -2506,7 +2506,7 @@
         <v>28</v>
       </c>
       <c r="C36" s="1">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D36" s="1">
         <v>5554</v>
@@ -2530,7 +2530,7 @@
         <v>12</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>12</v>
@@ -2548,7 +2548,7 @@
         <v>28</v>
       </c>
       <c r="C37" s="1">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="D37" s="1">
         <v>5554</v>
@@ -2590,7 +2590,7 @@
         <v>28</v>
       </c>
       <c r="C38" s="1">
-        <v>1652</v>
+        <v>1525</v>
       </c>
       <c r="D38" s="1">
         <v>5554</v>
@@ -2632,7 +2632,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="1">
-        <v>1702</v>
+        <v>1652</v>
       </c>
       <c r="D39" s="1">
         <v>5554</v>
@@ -2674,7 +2674,7 @@
         <v>28</v>
       </c>
       <c r="C40" s="1">
-        <v>1731</v>
+        <v>1702</v>
       </c>
       <c r="D40" s="1">
         <v>5554</v>
@@ -2710,19 +2710,19 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C41" s="1">
-        <v>1767</v>
+        <v>1731</v>
       </c>
       <c r="D41" s="1">
-        <v>4853</v>
+        <v>5554</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>12</v>
@@ -2734,7 +2734,7 @@
         <v>12</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>12</v>
@@ -2752,19 +2752,19 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C42" s="1">
         <v>1767</v>
       </c>
       <c r="D42" s="1">
-        <v>5653</v>
+        <v>4853</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>12</v>
@@ -2803,10 +2803,10 @@
         <v>1767</v>
       </c>
       <c r="D43" s="1">
-        <v>4914</v>
+        <v>5653</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>12</v>
@@ -2839,16 +2839,16 @@
         <v>16</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C44" s="1">
-        <v>1789</v>
+        <v>1767</v>
       </c>
       <c r="D44" s="1">
-        <v>5554</v>
+        <v>4914</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>12</v>
@@ -2860,7 +2860,7 @@
         <v>12</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>12</v>
@@ -2887,10 +2887,10 @@
         <v>1789</v>
       </c>
       <c r="D45" s="1">
-        <v>5662</v>
+        <v>5554</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>12</v>
@@ -2926,13 +2926,13 @@
         <v>28</v>
       </c>
       <c r="C46" s="1">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="D46" s="1">
-        <v>5554</v>
+        <v>5662</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>12</v>
@@ -2971,10 +2971,10 @@
         <v>1790</v>
       </c>
       <c r="D47" s="1">
-        <v>5662</v>
+        <v>5554</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>12</v>
@@ -3010,13 +3010,13 @@
         <v>28</v>
       </c>
       <c r="C48" s="1">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="D48" s="1">
-        <v>5554</v>
+        <v>5662</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>12</v>
@@ -3028,7 +3028,7 @@
         <v>12</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>12</v>
@@ -3052,7 +3052,7 @@
         <v>28</v>
       </c>
       <c r="C49" s="1">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="D49" s="1">
         <v>5554</v>
@@ -3094,7 +3094,7 @@
         <v>28</v>
       </c>
       <c r="C50" s="1">
-        <v>1813</v>
+        <v>1792</v>
       </c>
       <c r="D50" s="1">
         <v>5554</v>
@@ -3130,19 +3130,19 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C51" s="1">
-        <v>1819</v>
+        <v>1813</v>
       </c>
       <c r="D51" s="1">
-        <v>5458</v>
+        <v>5554</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>12</v>
@@ -3154,7 +3154,7 @@
         <v>12</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>12</v>
@@ -3168,25 +3168,23 @@
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
-      <c r="P51" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="P51" s="1"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C52" s="1">
         <v>1819</v>
       </c>
       <c r="D52" s="1">
-        <v>5526</v>
+        <v>5458</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>12</v>
@@ -3217,20 +3215,20 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>3</v>
+      <c r="A53" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C53" s="1">
         <v>1819</v>
       </c>
       <c r="D53" s="1">
-        <v>5550</v>
+        <v>5526</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>12</v>
@@ -3271,10 +3269,10 @@
         <v>1819</v>
       </c>
       <c r="D54" s="1">
-        <v>5677</v>
+        <v>5550</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>12</v>
@@ -3305,20 +3303,20 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>16</v>
+      <c r="A55" s="1">
+        <v>3</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C55" s="1">
         <v>1819</v>
       </c>
       <c r="D55" s="1">
-        <v>5623</v>
+        <v>5677</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>12</v>
@@ -3353,16 +3351,16 @@
         <v>16</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C56" s="1">
         <v>1819</v>
       </c>
       <c r="D56" s="1">
-        <v>5554</v>
+        <v>5623</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>12</v>
@@ -3397,16 +3395,16 @@
         <v>16</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C57" s="1">
         <v>1819</v>
       </c>
       <c r="D57" s="1">
-        <v>5900</v>
+        <v>5554</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>12</v>
@@ -3441,16 +3439,16 @@
         <v>16</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C58" s="1">
         <v>1819</v>
       </c>
       <c r="D58" s="1">
-        <v>5662</v>
+        <v>5900</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>12</v>
@@ -3488,13 +3486,13 @@
         <v>28</v>
       </c>
       <c r="C59" s="1">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="D59" s="1">
-        <v>5554</v>
+        <v>5662</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>12</v>
@@ -3520,26 +3518,28 @@
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
+      <c r="P59" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
-        <v>3</v>
+      <c r="A60" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C60" s="1">
-        <v>1830</v>
+        <v>1820</v>
       </c>
       <c r="D60" s="1">
-        <v>5434</v>
+        <v>5554</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>12</v>
@@ -3553,16 +3553,16 @@
       <c r="J60" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K60" s="1"/>
+      <c r="K60" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="L60" s="1" t="s">
         <v>12</v>
       </c>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
-      <c r="P60" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="P60" s="1"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
@@ -3575,13 +3575,13 @@
         <v>1830</v>
       </c>
       <c r="D61" s="1">
-        <v>5595</v>
+        <v>5434</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>12</v>
@@ -3595,9 +3595,7 @@
       <c r="J61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K61" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="K61" s="1"/>
       <c r="L61" s="1" t="s">
         <v>12</v>
       </c>
@@ -3619,10 +3617,10 @@
         <v>1830</v>
       </c>
       <c r="D62" s="1">
-        <v>5596</v>
+        <v>5595</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>12</v>
@@ -3639,7 +3637,9 @@
       <c r="J62" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K62" s="1"/>
+      <c r="K62" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="L62" s="1" t="s">
         <v>12</v>
       </c>
@@ -3651,20 +3651,20 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>16</v>
+      <c r="A63" s="1">
+        <v>3</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C63" s="1">
         <v>1830</v>
       </c>
       <c r="D63" s="1">
-        <v>5891</v>
+        <v>5596</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>12</v>
@@ -3681,9 +3681,7 @@
       <c r="J63" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K63" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="K63" s="1"/>
       <c r="L63" s="1" t="s">
         <v>12</v>
       </c>
@@ -3705,10 +3703,10 @@
         <v>1830</v>
       </c>
       <c r="D64" s="1">
-        <v>5900</v>
+        <v>5891</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>12</v>
@@ -3739,23 +3737,23 @@
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
-        <v>0</v>
+      <c r="A65" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C65" s="1">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="D65" s="1">
-        <v>5528</v>
+        <v>5900</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>12</v>
@@ -3764,7 +3762,7 @@
         <v>12</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>12</v>
@@ -3783,23 +3781,23 @@
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>16</v>
+      <c r="A66" s="1">
+        <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C66" s="1">
         <v>1831</v>
       </c>
       <c r="D66" s="1">
-        <v>5900</v>
+        <v>5528</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>12</v>
@@ -3831,16 +3829,16 @@
         <v>16</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C67" s="1">
         <v>1831</v>
       </c>
       <c r="D67" s="1">
-        <v>5662</v>
+        <v>5900</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>12</v>
@@ -3867,6 +3865,50 @@
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
       <c r="P67" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1831</v>
+      </c>
+      <c r="D68" s="1">
+        <v>5662</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3896,7 +3938,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
build after adding AM 1054
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_Geometry/Bugzilla_list.xlsx
+++ b/publication/part1000/CR_Geometry/Bugzilla_list.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="CR_geometry Bugs and Parts list" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs vs Parts Summary" sheetId="6" r:id="rId2"/>
-    <sheet name="Moved out from initial list" sheetId="2" r:id="rId3"/>
+    <sheet name="Removed from initial list" sheetId="2" r:id="rId3"/>
     <sheet name="Legend" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="103">
   <si>
     <t>Bug Description</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Add 3D Scan data to part 42</t>
   </si>
   <si>
-    <t>reopened</t>
-  </si>
-  <si>
     <t xml:space="preserve">yes </t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Add 3D Scan data AM</t>
   </si>
   <si>
-    <t>reopened, updated locally</t>
-  </si>
-  <si>
     <t>dispatched</t>
   </si>
   <si>
@@ -330,6 +324,21 @@
   </si>
   <si>
     <t>Collector bug for Part 42 Ed 5 for CR_Geometry</t>
+  </si>
+  <si>
+    <t>Collector bugs which has been declined for each modules</t>
+  </si>
+  <si>
+    <t>Modules moved out of scope</t>
+  </si>
+  <si>
+    <t>done locally</t>
+  </si>
+  <si>
+    <t>wg21</t>
+  </si>
+  <si>
+    <t>New positive_length_measure for the ARM</t>
   </si>
 </sst>
 </file>
@@ -371,8 +380,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color theme="5" tint="-0.499984740745262"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -398,7 +408,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -406,8 +416,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -957,33 +973,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="59.83203125" customWidth="1"/>
-    <col min="6" max="11" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="65.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="5" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" customWidth="1"/>
     <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="15" max="16" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>0</v>
@@ -1016,10 +1034,10 @@
         <v>9</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1063,7 +1081,9 @@
         <v>12</v>
       </c>
       <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="O2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1109,7 +1129,9 @@
         <v>12</v>
       </c>
       <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="O3" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1155,7 +1177,9 @@
         <v>12</v>
       </c>
       <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="O4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1177,7 +1201,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
@@ -1201,7 +1225,9 @@
         <v>12</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="O5" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1220,13 +1246,13 @@
         <v>5566</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>12</v>
@@ -1247,7 +1273,9 @@
         <v>12</v>
       </c>
       <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+      <c r="O6" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1257,7 +1285,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1">
         <v>42</v>
@@ -1266,7 +1294,7 @@
         <v>4861</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>12</v>
@@ -1293,7 +1321,9 @@
         <v>12</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+      <c r="O7" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1303,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1">
         <v>42</v>
@@ -1312,7 +1342,7 @@
         <v>5703</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>12</v>
@@ -1339,7 +1369,9 @@
         <v>12</v>
       </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="O8" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1349,7 +1381,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1">
         <v>42</v>
@@ -1358,7 +1390,7 @@
         <v>5650</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>12</v>
@@ -1385,7 +1417,9 @@
         <v>12</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
+      <c r="O9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1395,7 +1429,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1">
         <v>42</v>
@@ -1404,7 +1438,7 @@
         <v>5805</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>12</v>
@@ -1431,7 +1465,9 @@
         <v>12</v>
       </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="O10" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1441,7 +1477,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1">
         <v>42</v>
@@ -1450,7 +1486,7 @@
         <v>5650</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>12</v>
@@ -1477,7 +1513,9 @@
         <v>12</v>
       </c>
       <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+      <c r="O11" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1496,7 +1534,7 @@
         <v>5454</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>12</v>
@@ -1508,7 +1546,7 @@
         <v>12</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>12</v>
@@ -1523,7 +1561,9 @@
         <v>12</v>
       </c>
       <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
+      <c r="O12" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1533,7 +1573,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1">
         <v>43</v>
@@ -1542,7 +1582,7 @@
         <v>5806</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>12</v>
@@ -1554,7 +1594,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>12</v>
@@ -1569,7 +1609,9 @@
         <v>12</v>
       </c>
       <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
+      <c r="O13" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1579,7 +1621,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2">
         <v>409</v>
@@ -1588,10 +1630,10 @@
         <v>5898</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>12</v>
@@ -1600,24 +1642,30 @@
         <v>12</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M14" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="O14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2">
         <v>410</v>
@@ -1626,11 +1674,11 @@
         <v>5897</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1638,24 +1686,30 @@
         <v>12</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="1"/>
+      <c r="M15" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="O15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2">
         <v>442</v>
@@ -1664,10 +1718,10 @@
         <v>5896</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>12</v>
@@ -1676,24 +1730,30 @@
         <v>12</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M16" s="1"/>
+      <c r="M16" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="O16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1">
         <v>1004</v>
@@ -1702,7 +1762,7 @@
         <v>5605</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>12</v>
@@ -1725,17 +1785,23 @@
       <c r="L17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M17" s="1"/>
+      <c r="M17" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="O17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1">
         <v>1004</v>
@@ -1744,7 +1810,7 @@
         <v>5151</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>12</v>
@@ -1767,17 +1833,23 @@
       <c r="L18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="1"/>
+      <c r="M18" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="O18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1">
         <v>1004</v>
@@ -1786,7 +1858,7 @@
         <v>5662</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>12</v>
@@ -1809,10 +1881,16 @@
       <c r="L19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M19" s="1"/>
+      <c r="M19" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+      <c r="O19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1828,7 +1906,7 @@
         <v>5465</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>12</v>
@@ -1851,17 +1929,23 @@
       <c r="L20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M20" s="1"/>
+      <c r="M20" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="O20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1">
         <v>1004</v>
@@ -1870,7 +1954,7 @@
         <v>5217</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>12</v>
@@ -1893,17 +1977,23 @@
       <c r="L21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M21" s="1"/>
+      <c r="M21" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
+      <c r="O21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1">
         <v>1005</v>
@@ -1912,7 +2002,7 @@
         <v>5554</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>12</v>
@@ -1924,7 +2014,7 @@
         <v>12</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>12</v>
@@ -1935,17 +2025,23 @@
       <c r="L22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M22" s="1"/>
+      <c r="M22" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="O22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1">
         <v>1005</v>
@@ -1954,7 +2050,7 @@
         <v>5662</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>12</v>
@@ -1966,7 +2062,7 @@
         <v>12</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>12</v>
@@ -1977,26 +2073,32 @@
       <c r="L23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="1"/>
+      <c r="M23" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
+      <c r="O23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C24" s="1">
-        <v>1110</v>
+        <v>1054</v>
       </c>
       <c r="D24" s="1">
-        <v>5554</v>
+        <v>5524</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>12</v>
@@ -2008,7 +2110,7 @@
         <v>12</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>12</v>
@@ -2019,19 +2121,23 @@
       <c r="L24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M24" s="1"/>
+      <c r="M24" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
+      <c r="O24" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P24" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1">
         <v>1131</v>
@@ -2040,7 +2146,7 @@
         <v>5030</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>12</v>
@@ -2052,7 +2158,7 @@
         <v>12</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>12</v>
@@ -2065,15 +2171,19 @@
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
+      <c r="O25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1">
         <v>1131</v>
@@ -2082,7 +2192,7 @@
         <v>5554</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>12</v>
@@ -2094,7 +2204,7 @@
         <v>12</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>12</v>
@@ -2105,10 +2215,16 @@
       <c r="L26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M26" s="1"/>
+      <c r="M26" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
+      <c r="O26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -2124,7 +2240,7 @@
         <v>5509</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>12</v>
@@ -2136,7 +2252,7 @@
         <v>12</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>12</v>
@@ -2145,11 +2261,15 @@
         <v>12</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M27" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
+      <c r="O27" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P27" s="1" t="s">
         <v>12</v>
       </c>
@@ -2159,7 +2279,7 @@
         <v>16</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1">
         <v>1319</v>
@@ -2168,7 +2288,7 @@
         <v>5662</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>12</v>
@@ -2180,7 +2300,7 @@
         <v>12</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>12</v>
@@ -2191,17 +2311,23 @@
       <c r="L28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M28" s="1"/>
+      <c r="M28" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
+      <c r="O28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1">
         <v>1507</v>
@@ -2210,7 +2336,7 @@
         <v>5554</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>12</v>
@@ -2222,7 +2348,7 @@
         <v>12</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>12</v>
@@ -2233,17 +2359,23 @@
       <c r="L29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M29" s="1"/>
+      <c r="M29" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
+      <c r="O29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30" s="1">
         <v>1507</v>
@@ -2252,7 +2384,7 @@
         <v>5662</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>12</v>
@@ -2264,7 +2396,7 @@
         <v>12</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>12</v>
@@ -2275,17 +2407,23 @@
       <c r="L30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M30" s="1"/>
+      <c r="M30" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
+      <c r="O30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C31" s="1">
         <v>1509</v>
@@ -2294,7 +2432,7 @@
         <v>5554</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>12</v>
@@ -2306,7 +2444,7 @@
         <v>12</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>12</v>
@@ -2317,17 +2455,23 @@
       <c r="L31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M31" s="1"/>
+      <c r="M31" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
+      <c r="O31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1">
         <v>1514</v>
@@ -2336,7 +2480,7 @@
         <v>5554</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>12</v>
@@ -2348,7 +2492,7 @@
         <v>12</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>12</v>
@@ -2359,10 +2503,16 @@
       <c r="L32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="1"/>
+      <c r="M32" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
+      <c r="O32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -2378,7 +2528,7 @@
         <v>5630</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>12</v>
@@ -2390,7 +2540,7 @@
         <v>12</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>12</v>
@@ -2405,7 +2555,9 @@
         <v>12</v>
       </c>
       <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
+      <c r="O33" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P33" s="1" t="s">
         <v>12</v>
       </c>
@@ -2415,7 +2567,7 @@
         <v>16</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C34" s="1">
         <v>1520</v>
@@ -2424,20 +2576,20 @@
         <v>5554</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="J34" s="1" t="s">
         <v>12</v>
       </c>
@@ -2451,7 +2603,9 @@
         <v>12</v>
       </c>
       <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
+      <c r="O34" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P34" s="1" t="s">
         <v>12</v>
       </c>
@@ -2461,7 +2615,7 @@
         <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1">
         <v>1521</v>
@@ -2470,7 +2624,7 @@
         <v>5554</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>12</v>
@@ -2482,7 +2636,7 @@
         <v>12</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>12</v>
@@ -2493,17 +2647,23 @@
       <c r="L35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M35" s="1"/>
+      <c r="M35" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
+      <c r="O35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C36" s="1">
         <v>1522</v>
@@ -2512,7 +2672,7 @@
         <v>5554</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>12</v>
@@ -2524,28 +2684,34 @@
         <v>12</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M36" s="1"/>
+      <c r="M36" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
+      <c r="O36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C37" s="1">
         <v>1523</v>
@@ -2554,7 +2720,7 @@
         <v>5554</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>12</v>
@@ -2566,7 +2732,7 @@
         <v>12</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>12</v>
@@ -2577,17 +2743,23 @@
       <c r="L37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M37" s="1"/>
+      <c r="M37" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
+      <c r="O37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C38" s="1">
         <v>1525</v>
@@ -2596,7 +2768,7 @@
         <v>5554</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>12</v>
@@ -2608,7 +2780,7 @@
         <v>12</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>12</v>
@@ -2619,17 +2791,23 @@
       <c r="L38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M38" s="1"/>
+      <c r="M38" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
+      <c r="O38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C39" s="1">
         <v>1652</v>
@@ -2638,7 +2816,7 @@
         <v>5554</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>12</v>
@@ -2650,7 +2828,7 @@
         <v>12</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>12</v>
@@ -2661,17 +2839,23 @@
       <c r="L39" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M39" s="1"/>
+      <c r="M39" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
+      <c r="O39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C40" s="1">
         <v>1702</v>
@@ -2680,7 +2864,7 @@
         <v>5554</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>12</v>
@@ -2692,7 +2876,7 @@
         <v>12</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>12</v>
@@ -2703,17 +2887,23 @@
       <c r="L40" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M40" s="1"/>
+      <c r="M40" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
+      <c r="O40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C41" s="1">
         <v>1731</v>
@@ -2722,7 +2912,7 @@
         <v>5554</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>12</v>
@@ -2734,7 +2924,7 @@
         <v>12</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>12</v>
@@ -2745,17 +2935,23 @@
       <c r="L41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M41" s="1"/>
+      <c r="M41" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
+      <c r="O41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C42" s="1">
         <v>1767</v>
@@ -2764,7 +2960,7 @@
         <v>4853</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>12</v>
@@ -2787,17 +2983,23 @@
       <c r="L42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M42" s="1"/>
+      <c r="M42" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
+      <c r="O42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C43" s="1">
         <v>1767</v>
@@ -2806,7 +3008,7 @@
         <v>5653</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>12</v>
@@ -2829,17 +3031,23 @@
       <c r="L43" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M43" s="1"/>
+      <c r="M43" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
+      <c r="O43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C44" s="1">
         <v>1767</v>
@@ -2848,7 +3056,7 @@
         <v>4914</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>12</v>
@@ -2871,17 +3079,23 @@
       <c r="L44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M44" s="1"/>
+      <c r="M44" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
+      <c r="O44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C45" s="1">
         <v>1789</v>
@@ -2890,20 +3104,20 @@
         <v>5554</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="J45" s="1" t="s">
         <v>12</v>
       </c>
@@ -2913,17 +3127,23 @@
       <c r="L45" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M45" s="1"/>
+      <c r="M45" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
+      <c r="O45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C46" s="1">
         <v>1789</v>
@@ -2932,7 +3152,7 @@
         <v>5662</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>12</v>
@@ -2944,7 +3164,7 @@
         <v>12</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>12</v>
@@ -2955,17 +3175,23 @@
       <c r="L46" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M46" s="1"/>
+      <c r="M46" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
+      <c r="O46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C47" s="1">
         <v>1790</v>
@@ -2974,20 +3200,20 @@
         <v>5554</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="J47" s="1" t="s">
         <v>12</v>
       </c>
@@ -2997,17 +3223,23 @@
       <c r="L47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M47" s="1"/>
+      <c r="M47" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
+      <c r="O47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C48" s="1">
         <v>1790</v>
@@ -3016,7 +3248,7 @@
         <v>5662</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>12</v>
@@ -3028,7 +3260,7 @@
         <v>12</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>12</v>
@@ -3039,17 +3271,23 @@
       <c r="L48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M48" s="1"/>
+      <c r="M48" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
+      <c r="O48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C49" s="1">
         <v>1791</v>
@@ -3058,7 +3296,7 @@
         <v>5554</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>12</v>
@@ -3070,7 +3308,7 @@
         <v>12</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>12</v>
@@ -3081,17 +3319,23 @@
       <c r="L49" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M49" s="1"/>
+      <c r="M49" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
+      <c r="O49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C50" s="1">
         <v>1792</v>
@@ -3100,7 +3344,7 @@
         <v>5554</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>12</v>
@@ -3112,7 +3356,7 @@
         <v>12</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>12</v>
@@ -3123,17 +3367,23 @@
       <c r="L50" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M50" s="1"/>
+      <c r="M50" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
+      <c r="O50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C51" s="1">
         <v>1813</v>
@@ -3142,7 +3392,7 @@
         <v>5554</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>12</v>
@@ -3154,7 +3404,7 @@
         <v>12</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>12</v>
@@ -3165,17 +3415,23 @@
       <c r="L51" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M51" s="1"/>
+      <c r="M51" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
+      <c r="O51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C52" s="1">
         <v>1819</v>
@@ -3184,7 +3440,7 @@
         <v>5458</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>12</v>
@@ -3207,19 +3463,23 @@
       <c r="L52" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M52" s="1"/>
+      <c r="M52" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
+      <c r="O52" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P52" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C53" s="1">
         <v>1819</v>
@@ -3228,7 +3488,7 @@
         <v>5526</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>12</v>
@@ -3251,9 +3511,13 @@
       <c r="L53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M53" s="1"/>
+      <c r="M53" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
+      <c r="O53" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P53" s="1" t="s">
         <v>12</v>
       </c>
@@ -3272,7 +3536,7 @@
         <v>5550</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>12</v>
@@ -3295,9 +3559,13 @@
       <c r="L54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M54" s="1"/>
+      <c r="M54" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
+      <c r="O54" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P54" s="1" t="s">
         <v>12</v>
       </c>
@@ -3316,7 +3584,7 @@
         <v>5677</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>12</v>
@@ -3339,9 +3607,13 @@
       <c r="L55" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M55" s="1"/>
+      <c r="M55" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
+      <c r="O55" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P55" s="1" t="s">
         <v>12</v>
       </c>
@@ -3351,7 +3623,7 @@
         <v>16</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C56" s="1">
         <v>1819</v>
@@ -3360,7 +3632,7 @@
         <v>5623</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>12</v>
@@ -3383,9 +3655,13 @@
       <c r="L56" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M56" s="1"/>
+      <c r="M56" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
+      <c r="O56" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P56" s="1" t="s">
         <v>12</v>
       </c>
@@ -3395,7 +3671,7 @@
         <v>16</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C57" s="1">
         <v>1819</v>
@@ -3404,7 +3680,7 @@
         <v>5554</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>12</v>
@@ -3427,9 +3703,13 @@
       <c r="L57" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M57" s="1"/>
+      <c r="M57" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
+      <c r="O57" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P57" s="1" t="s">
         <v>12</v>
       </c>
@@ -3439,7 +3719,7 @@
         <v>16</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C58" s="1">
         <v>1819</v>
@@ -3448,7 +3728,7 @@
         <v>5900</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>12</v>
@@ -3471,9 +3751,13 @@
       <c r="L58" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M58" s="1"/>
+      <c r="M58" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
+      <c r="O58" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P58" s="1" t="s">
         <v>12</v>
       </c>
@@ -3483,7 +3767,7 @@
         <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C59" s="1">
         <v>1819</v>
@@ -3492,7 +3776,7 @@
         <v>5662</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>12</v>
@@ -3515,9 +3799,13 @@
       <c r="L59" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M59" s="1"/>
+      <c r="M59" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
+      <c r="O59" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P59" s="1" t="s">
         <v>12</v>
       </c>
@@ -3527,7 +3815,7 @@
         <v>16</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C60" s="1">
         <v>1820</v>
@@ -3536,7 +3824,7 @@
         <v>5554</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>12</v>
@@ -3559,10 +3847,16 @@
       <c r="L60" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M60" s="1"/>
+      <c r="M60" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
+      <c r="O60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
@@ -3578,10 +3872,10 @@
         <v>5434</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>12</v>
@@ -3599,9 +3893,13 @@
       <c r="L61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M61" s="1"/>
+      <c r="M61" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
+      <c r="O61" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P61" s="1" t="s">
         <v>12</v>
       </c>
@@ -3620,7 +3918,7 @@
         <v>5595</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>12</v>
@@ -3643,9 +3941,13 @@
       <c r="L62" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M62" s="1"/>
+      <c r="M62" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
+      <c r="O62" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P62" s="1" t="s">
         <v>12</v>
       </c>
@@ -3664,7 +3966,7 @@
         <v>5596</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>12</v>
@@ -3685,9 +3987,13 @@
       <c r="L63" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M63" s="1"/>
+      <c r="M63" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
+      <c r="O63" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P63" s="1" t="s">
         <v>12</v>
       </c>
@@ -3697,7 +4003,7 @@
         <v>16</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C64" s="1">
         <v>1830</v>
@@ -3706,7 +4012,7 @@
         <v>5891</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>12</v>
@@ -3729,9 +4035,13 @@
       <c r="L64" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M64" s="1"/>
+      <c r="M64" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
+      <c r="O64" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P64" s="1" t="s">
         <v>12</v>
       </c>
@@ -3741,7 +4051,7 @@
         <v>16</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C65" s="1">
         <v>1830</v>
@@ -3750,7 +4060,7 @@
         <v>5900</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>12</v>
@@ -3773,9 +4083,13 @@
       <c r="L65" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M65" s="1"/>
+      <c r="M65" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
+      <c r="O65" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P65" s="1" t="s">
         <v>12</v>
       </c>
@@ -3785,7 +4099,7 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C66" s="1">
         <v>1831</v>
@@ -3794,10 +4108,10 @@
         <v>5528</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>12</v>
@@ -3806,7 +4120,7 @@
         <v>12</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>12</v>
@@ -3817,9 +4131,13 @@
       <c r="L66" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M66" s="1"/>
+      <c r="M66" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
+      <c r="O66" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P66" s="1" t="s">
         <v>12</v>
       </c>
@@ -3829,7 +4147,7 @@
         <v>16</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C67" s="1">
         <v>1831</v>
@@ -3838,7 +4156,7 @@
         <v>5900</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>12</v>
@@ -3850,7 +4168,7 @@
         <v>12</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>12</v>
@@ -3861,9 +4179,13 @@
       <c r="L67" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M67" s="1"/>
+      <c r="M67" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
+      <c r="O67" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P67" s="1" t="s">
         <v>12</v>
       </c>
@@ -3873,7 +4195,7 @@
         <v>16</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C68" s="1">
         <v>1831</v>
@@ -3882,7 +4204,7 @@
         <v>5662</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>12</v>
@@ -3894,7 +4216,7 @@
         <v>12</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>12</v>
@@ -3905,9 +4227,13 @@
       <c r="L68" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M68" s="1"/>
+      <c r="M68" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
+      <c r="O68" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="P68" s="1" t="s">
         <v>12</v>
       </c>
@@ -3935,162 +4261,218 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E17" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="43.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="99.33203125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:16" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5554</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5644</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5662</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1386</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4987</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="1">
+      <c r="C8" s="6">
+        <v>1386</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5673</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1110</v>
+      </c>
+      <c r="D9" s="1">
         <v>5554</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5644</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5662</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1386</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4987</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1386</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5673</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4114,10 +4496,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4125,31 +4507,31 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -4157,7 +4539,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added pivot table for reporting
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_Geometry/Bugzilla_list.xlsx
+++ b/publication/part1000/CR_Geometry/Bugzilla_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="-18460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="1200" yWindow="-18460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CR_geometry Bugs and Parts list" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Legend" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="8" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="111">
   <si>
     <t>Bug Description</t>
   </si>
@@ -339,6 +342,30 @@
   </si>
   <si>
     <t>New positive_length_measure for the ARM</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Parts</t>
+  </si>
+  <si>
+    <t>Count of Bugs</t>
+  </si>
+  <si>
+    <t>3 lf schemas updated by CR</t>
+  </si>
+  <si>
+    <t>30 parts in CR</t>
+  </si>
+  <si>
+    <t>incl 2 ressources part</t>
+  </si>
+  <si>
+    <t>incl 28 AM</t>
   </si>
 </sst>
 </file>
@@ -408,7 +435,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -423,6 +450,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -678,6 +713,789 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Kevin Le Tutour" refreshedDate="42482.463360185182" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="67">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1[[Parts]:[Bugs]]"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="Parts" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="42" maxValue="1831" count="32">
+        <n v="42"/>
+        <n v="43"/>
+        <n v="409"/>
+        <n v="410"/>
+        <n v="442"/>
+        <n v="1004"/>
+        <n v="1005"/>
+        <n v="1054"/>
+        <n v="1131"/>
+        <n v="1318"/>
+        <n v="1319"/>
+        <n v="1507"/>
+        <n v="1509"/>
+        <n v="1514"/>
+        <n v="1520"/>
+        <n v="1521"/>
+        <n v="1522"/>
+        <n v="1523"/>
+        <n v="1525"/>
+        <n v="1652"/>
+        <n v="1702"/>
+        <n v="1731"/>
+        <n v="1767"/>
+        <n v="1789"/>
+        <n v="1790"/>
+        <n v="1791"/>
+        <n v="1792"/>
+        <n v="1813"/>
+        <n v="1819"/>
+        <n v="1820"/>
+        <n v="1830"/>
+        <n v="1831"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Bugs" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4853" maxValue="5900" count="39">
+        <n v="5409"/>
+        <n v="5448"/>
+        <n v="5452"/>
+        <n v="5527"/>
+        <n v="5566"/>
+        <n v="4861"/>
+        <n v="5703"/>
+        <n v="5185"/>
+        <n v="5805"/>
+        <n v="5650"/>
+        <n v="5454"/>
+        <n v="5806"/>
+        <n v="5898"/>
+        <n v="5897"/>
+        <n v="5896"/>
+        <n v="5605"/>
+        <n v="5151"/>
+        <n v="5662"/>
+        <n v="5465"/>
+        <n v="5217"/>
+        <n v="5554"/>
+        <n v="5524"/>
+        <n v="5030"/>
+        <n v="5509"/>
+        <n v="5630"/>
+        <n v="4853"/>
+        <n v="5653"/>
+        <n v="4914"/>
+        <n v="5458"/>
+        <n v="5526"/>
+        <n v="5550"/>
+        <n v="5677"/>
+        <n v="5623"/>
+        <n v="5900"/>
+        <n v="5434"/>
+        <n v="5595"/>
+        <n v="5596"/>
+        <n v="5891"/>
+        <n v="5528"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="67">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="23"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="25"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="26"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="27"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="28"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="29"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="30"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="31"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="32"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="34"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="35"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="36"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="37"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <x v="38"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <x v="17"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:C101" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="33">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="40">
+        <item x="25"/>
+        <item x="5"/>
+        <item x="27"/>
+        <item x="22"/>
+        <item x="16"/>
+        <item x="19"/>
+        <item x="0"/>
+        <item x="34"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="10"/>
+        <item x="28"/>
+        <item x="18"/>
+        <item x="23"/>
+        <item x="21"/>
+        <item x="29"/>
+        <item x="3"/>
+        <item x="38"/>
+        <item x="30"/>
+        <item x="20"/>
+        <item x="4"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="15"/>
+        <item x="32"/>
+        <item x="24"/>
+        <item x="9"/>
+        <item x="26"/>
+        <item x="17"/>
+        <item x="31"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="37"/>
+        <item x="14"/>
+        <item x="13"/>
+        <item x="12"/>
+        <item x="33"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="100">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="30"/>
+    </i>
+    <i r="1">
+      <x v="31"/>
+    </i>
+    <i r="1">
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="29"/>
+    </i>
+    <i r="1">
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="33"/>
+    </i>
+    <i r="1">
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="37"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of Parts" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of Bugs" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -973,8 +1791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1387,7 +2205,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="1">
-        <v>5650</v>
+        <v>5185</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>83</v>
@@ -4249,12 +5067,1151 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>42</v>
+      </c>
+      <c r="B2" s="9">
+        <v>10</v>
+      </c>
+      <c r="C2" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <v>4861</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>5409</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="12">
+        <v>5448</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <v>5452</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
+        <v>5527</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>5566</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
+        <v>5650</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>5703</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>5805</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>5185</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>43</v>
+      </c>
+      <c r="B13" s="9">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="12">
+        <v>5454</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="12">
+        <v>5806</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>409</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="12">
+        <v>5898</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>410</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="12">
+        <v>5897</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <v>442</v>
+      </c>
+      <c r="B20" s="9">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="12">
+        <v>5896</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="11">
+        <v>1004</v>
+      </c>
+      <c r="B22" s="9">
+        <v>5</v>
+      </c>
+      <c r="C22" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="12">
+        <v>5151</v>
+      </c>
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="12">
+        <v>5217</v>
+      </c>
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="12">
+        <v>5465</v>
+      </c>
+      <c r="B25" s="9">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="12">
+        <v>5605</v>
+      </c>
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+      <c r="C26" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="12">
+        <v>5662</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="11">
+        <v>1005</v>
+      </c>
+      <c r="B28" s="9">
+        <v>2</v>
+      </c>
+      <c r="C28" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B29" s="9">
+        <v>1</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="12">
+        <v>5662</v>
+      </c>
+      <c r="B30" s="9">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="11">
+        <v>1054</v>
+      </c>
+      <c r="B31" s="9">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="12">
+        <v>5524</v>
+      </c>
+      <c r="B32" s="9">
+        <v>1</v>
+      </c>
+      <c r="C32" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="11">
+        <v>1131</v>
+      </c>
+      <c r="B33" s="9">
+        <v>2</v>
+      </c>
+      <c r="C33" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="12">
+        <v>5030</v>
+      </c>
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B35" s="9">
+        <v>1</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="11">
+        <v>1318</v>
+      </c>
+      <c r="B36" s="9">
+        <v>1</v>
+      </c>
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="12">
+        <v>5509</v>
+      </c>
+      <c r="B37" s="9">
+        <v>1</v>
+      </c>
+      <c r="C37" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="11">
+        <v>1319</v>
+      </c>
+      <c r="B38" s="9">
+        <v>1</v>
+      </c>
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="12">
+        <v>5662</v>
+      </c>
+      <c r="B39" s="9">
+        <v>1</v>
+      </c>
+      <c r="C39" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="11">
+        <v>1507</v>
+      </c>
+      <c r="B40" s="9">
+        <v>2</v>
+      </c>
+      <c r="C40" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B41" s="9">
+        <v>1</v>
+      </c>
+      <c r="C41" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="12">
+        <v>5662</v>
+      </c>
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="11">
+        <v>1509</v>
+      </c>
+      <c r="B43" s="9">
+        <v>1</v>
+      </c>
+      <c r="C43" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B44" s="9">
+        <v>1</v>
+      </c>
+      <c r="C44" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="11">
+        <v>1514</v>
+      </c>
+      <c r="B45" s="9">
+        <v>1</v>
+      </c>
+      <c r="C45" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B46" s="9">
+        <v>1</v>
+      </c>
+      <c r="C46" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="11">
+        <v>1520</v>
+      </c>
+      <c r="B47" s="9">
+        <v>2</v>
+      </c>
+      <c r="C47" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B48" s="9">
+        <v>1</v>
+      </c>
+      <c r="C48" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="12">
+        <v>5630</v>
+      </c>
+      <c r="B49" s="9">
+        <v>1</v>
+      </c>
+      <c r="C49" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="11">
+        <v>1521</v>
+      </c>
+      <c r="B50" s="9">
+        <v>1</v>
+      </c>
+      <c r="C50" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B51" s="9">
+        <v>1</v>
+      </c>
+      <c r="C51" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="11">
+        <v>1522</v>
+      </c>
+      <c r="B52" s="9">
+        <v>1</v>
+      </c>
+      <c r="C52" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B53" s="9">
+        <v>1</v>
+      </c>
+      <c r="C53" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="11">
+        <v>1523</v>
+      </c>
+      <c r="B54" s="9">
+        <v>1</v>
+      </c>
+      <c r="C54" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B55" s="9">
+        <v>1</v>
+      </c>
+      <c r="C55" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="11">
+        <v>1525</v>
+      </c>
+      <c r="B56" s="9">
+        <v>1</v>
+      </c>
+      <c r="C56" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B57" s="9">
+        <v>1</v>
+      </c>
+      <c r="C57" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="11">
+        <v>1652</v>
+      </c>
+      <c r="B58" s="9">
+        <v>1</v>
+      </c>
+      <c r="C58" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B59" s="9">
+        <v>1</v>
+      </c>
+      <c r="C59" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="11">
+        <v>1702</v>
+      </c>
+      <c r="B60" s="9">
+        <v>1</v>
+      </c>
+      <c r="C60" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B61" s="9">
+        <v>1</v>
+      </c>
+      <c r="C61" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="11">
+        <v>1731</v>
+      </c>
+      <c r="B62" s="9">
+        <v>1</v>
+      </c>
+      <c r="C62" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B63" s="9">
+        <v>1</v>
+      </c>
+      <c r="C63" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="11">
+        <v>1767</v>
+      </c>
+      <c r="B64" s="9">
+        <v>3</v>
+      </c>
+      <c r="C64" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="12">
+        <v>4853</v>
+      </c>
+      <c r="B65" s="9">
+        <v>1</v>
+      </c>
+      <c r="C65" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="12">
+        <v>4914</v>
+      </c>
+      <c r="B66" s="9">
+        <v>1</v>
+      </c>
+      <c r="C66" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="12">
+        <v>5653</v>
+      </c>
+      <c r="B67" s="9">
+        <v>1</v>
+      </c>
+      <c r="C67" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="11">
+        <v>1789</v>
+      </c>
+      <c r="B68" s="9">
+        <v>2</v>
+      </c>
+      <c r="C68" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B69" s="9">
+        <v>1</v>
+      </c>
+      <c r="C69" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="12">
+        <v>5662</v>
+      </c>
+      <c r="B70" s="9">
+        <v>1</v>
+      </c>
+      <c r="C70" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="11">
+        <v>1790</v>
+      </c>
+      <c r="B71" s="9">
+        <v>2</v>
+      </c>
+      <c r="C71" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B72" s="9">
+        <v>1</v>
+      </c>
+      <c r="C72" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="12">
+        <v>5662</v>
+      </c>
+      <c r="B73" s="9">
+        <v>1</v>
+      </c>
+      <c r="C73" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="11">
+        <v>1791</v>
+      </c>
+      <c r="B74" s="9">
+        <v>1</v>
+      </c>
+      <c r="C74" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B75" s="9">
+        <v>1</v>
+      </c>
+      <c r="C75" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="11">
+        <v>1792</v>
+      </c>
+      <c r="B76" s="9">
+        <v>1</v>
+      </c>
+      <c r="C76" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B77" s="9">
+        <v>1</v>
+      </c>
+      <c r="C77" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="11">
+        <v>1813</v>
+      </c>
+      <c r="B78" s="9">
+        <v>1</v>
+      </c>
+      <c r="C78" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B79" s="9">
+        <v>1</v>
+      </c>
+      <c r="C79" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="11">
+        <v>1819</v>
+      </c>
+      <c r="B80" s="9">
+        <v>8</v>
+      </c>
+      <c r="C80" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="12">
+        <v>5458</v>
+      </c>
+      <c r="B81" s="9">
+        <v>1</v>
+      </c>
+      <c r="C81" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="12">
+        <v>5526</v>
+      </c>
+      <c r="B82" s="9">
+        <v>1</v>
+      </c>
+      <c r="C82" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="12">
+        <v>5550</v>
+      </c>
+      <c r="B83" s="9">
+        <v>1</v>
+      </c>
+      <c r="C83" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B84" s="9">
+        <v>1</v>
+      </c>
+      <c r="C84" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="12">
+        <v>5623</v>
+      </c>
+      <c r="B85" s="9">
+        <v>1</v>
+      </c>
+      <c r="C85" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="12">
+        <v>5662</v>
+      </c>
+      <c r="B86" s="9">
+        <v>1</v>
+      </c>
+      <c r="C86" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="12">
+        <v>5677</v>
+      </c>
+      <c r="B87" s="9">
+        <v>1</v>
+      </c>
+      <c r="C87" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="12">
+        <v>5900</v>
+      </c>
+      <c r="B88" s="9">
+        <v>1</v>
+      </c>
+      <c r="C88" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="11">
+        <v>1820</v>
+      </c>
+      <c r="B89" s="9">
+        <v>1</v>
+      </c>
+      <c r="C89" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="12">
+        <v>5554</v>
+      </c>
+      <c r="B90" s="9">
+        <v>1</v>
+      </c>
+      <c r="C90" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="11">
+        <v>1830</v>
+      </c>
+      <c r="B91" s="9">
+        <v>5</v>
+      </c>
+      <c r="C91" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="12">
+        <v>5434</v>
+      </c>
+      <c r="B92" s="9">
+        <v>1</v>
+      </c>
+      <c r="C92" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="12">
+        <v>5595</v>
+      </c>
+      <c r="B93" s="9">
+        <v>1</v>
+      </c>
+      <c r="C93" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="12">
+        <v>5596</v>
+      </c>
+      <c r="B94" s="9">
+        <v>1</v>
+      </c>
+      <c r="C94" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="12">
+        <v>5891</v>
+      </c>
+      <c r="B95" s="9">
+        <v>1</v>
+      </c>
+      <c r="C95" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="12">
+        <v>5900</v>
+      </c>
+      <c r="B96" s="9">
+        <v>1</v>
+      </c>
+      <c r="C96" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="11">
+        <v>1831</v>
+      </c>
+      <c r="B97" s="9">
+        <v>3</v>
+      </c>
+      <c r="C97" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="12">
+        <v>5528</v>
+      </c>
+      <c r="B98" s="9">
+        <v>1</v>
+      </c>
+      <c r="C98" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="12">
+        <v>5662</v>
+      </c>
+      <c r="B99" s="9">
+        <v>1</v>
+      </c>
+      <c r="C99" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="12">
+        <v>5900</v>
+      </c>
+      <c r="B100" s="9">
+        <v>1</v>
+      </c>
+      <c r="C100" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101" s="9">
+        <v>67</v>
+      </c>
+      <c r="C101" s="9">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>